<commit_message>
Project Case52 is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/Case52/module1.xlsx
+++ b/Case52/module1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case5/base/"/>
     </mc:Choice>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -338,16 +338,20 @@
   </si>
   <si>
     <t>VT</t>
+  </si>
+  <si>
+    <t>Data MyDatatype Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,14 +359,14 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Monaco"/>
       <family val="2"/>
     </font>
@@ -416,7 +420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4472C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +644,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1076,7 +1080,7 @@
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>

</xml_diff>